<commit_message>
working first two dropdowns
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/exams.xlsx
+++ b/app/src/main/res/raw/exams.xlsx
@@ -159,7 +159,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -220,10 +220,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal 2" xfId="1"/>

</xml_diff>